<commit_message>
Porcentagem do resultado quiz
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B73835C-E6E4-437A-8E69-B3A6655E80B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shocker\Desktop\SpTech\Pesquisa e Inovação\Projeto Individual\ProjetoIndividual\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4085FB12-10B4-4671-BF51-E288F28031C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="89">
   <si>
     <t>OBS: Essa tabela está sujeita a alterações, podendo ter seus dados modificados, incrementados ou removidos com o decorrer do projeto.</t>
   </si>
@@ -307,12 +312,15 @@
   <si>
     <t>SP4</t>
   </si>
+  <si>
+    <t>5.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,6 +725,138 @@
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,138 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,7 +896,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1186,547 +1194,556 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
     <col min="8" max="8" width="36" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:12">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="6" spans="4:12">
-      <c r="D6" s="4" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D6" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="4:12">
-      <c r="D7" s="8" t="s">
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="4:12" ht="45.75">
-      <c r="D8" s="12">
+    <row r="8" spans="4:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D8" s="35">
         <v>1</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="35">
         <v>8</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="4:12" ht="60.75">
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20" t="s">
+    <row r="9" spans="4:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="36"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="4:12" ht="135" customHeight="1">
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="38"/>
+    </row>
+    <row r="10" spans="4:12" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="36"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="11" spans="4:12" ht="138.75" customHeight="1">
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20" t="s">
+      <c r="I10" s="36"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="38"/>
+    </row>
+    <row r="11" spans="4:12" ht="138.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="36"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="23"/>
-    </row>
-    <row r="12" spans="4:12" ht="100.5" customHeight="1">
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="25" t="s">
+      <c r="I11" s="36"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="38"/>
+    </row>
+    <row r="12" spans="4:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="36"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="13" spans="4:12" ht="139.5" customHeight="1">
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="14" t="s">
+      <c r="I12" s="36"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="38"/>
+    </row>
+    <row r="13" spans="4:12" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="36"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="35">
         <v>13</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="4:12" ht="156.75" customHeight="1">
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20" t="s">
+    <row r="14" spans="4:12" ht="156.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="36"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="23"/>
-    </row>
-    <row r="15" spans="4:12" ht="183" customHeight="1">
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="25" t="s">
+      <c r="I14" s="36"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="38"/>
+    </row>
+    <row r="15" spans="4:12" ht="183" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="36"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="4:12" ht="178.5" customHeight="1">
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="14" t="s">
+      <c r="I15" s="36"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="38"/>
+    </row>
+    <row r="16" spans="4:12" ht="178.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="36"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="35">
         <v>13</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="4:12" ht="144" customHeight="1">
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="28" t="s">
+    <row r="17" spans="4:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="36"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="4:12" ht="60.75">
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="30" t="s">
+      <c r="I17" s="36"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="4:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="36"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="4:12" ht="129" customHeight="1">
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="14" t="s">
+      <c r="I18" s="36"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="38"/>
+    </row>
+    <row r="19" spans="4:12" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="36"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="35">
         <v>21</v>
       </c>
-      <c r="L19" s="17" t="s">
+      <c r="L19" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="180.75" customHeight="1">
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="28" t="s">
+    <row r="20" spans="4:12" ht="180.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="36"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="4:12" ht="117" customHeight="1">
-      <c r="D21" s="33">
+      <c r="I20" s="36"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="38"/>
+    </row>
+    <row r="21" spans="4:12" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="41">
         <v>2</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="K21" s="36">
+      <c r="K21" s="21">
         <v>8</v>
       </c>
-      <c r="L21" s="39" t="s">
+      <c r="L21" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="4:12" ht="135" customHeight="1">
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="14" t="s">
+    <row r="22" spans="4:12" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="36"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="35">
         <v>13</v>
       </c>
-      <c r="L22" s="17" t="s">
+      <c r="L22" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="4:12" ht="184.5" customHeight="1">
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="28" t="s">
+    <row r="23" spans="4:12" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="36"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="4:12" ht="165" customHeight="1">
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="28" t="s">
+      <c r="I23" s="36"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="38"/>
+    </row>
+    <row r="24" spans="4:12" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="36"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="23"/>
-    </row>
-    <row r="25" spans="4:12" ht="162" customHeight="1">
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="28" t="s">
+      <c r="I24" s="36"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="38"/>
+    </row>
+    <row r="25" spans="4:12" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="36"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="23"/>
-    </row>
-    <row r="26" spans="4:12" ht="117" customHeight="1">
-      <c r="D26" s="33">
+      <c r="I25" s="36"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="38"/>
+    </row>
+    <row r="26" spans="4:12" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="41">
         <v>4</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="I26" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="35">
         <v>13</v>
       </c>
-      <c r="L26" s="17" t="s">
+      <c r="L26" s="37" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="4:12" ht="216.75" customHeight="1">
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="20" t="s">
+    <row r="27" spans="4:12" ht="216.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="23"/>
-    </row>
-    <row r="28" spans="4:12" ht="45.75">
-      <c r="D28" s="18">
+      <c r="I27" s="36"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="38"/>
+    </row>
+    <row r="28" spans="4:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D28" s="36">
         <v>5</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="47" t="s">
+      <c r="F28" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="G28" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="51" t="s">
+      <c r="H28" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="K28" s="48">
+      <c r="K28" s="31">
         <v>3</v>
       </c>
-      <c r="L28" s="49" t="s">
+      <c r="L28" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="252.75" customHeight="1">
-      <c r="D29" s="43"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="40">
-        <v>5.2</v>
-      </c>
-      <c r="G29" s="41" t="s">
+    <row r="29" spans="4:12" ht="252.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="42" t="s">
+      <c r="H29" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="I29" s="41" t="s">
+      <c r="I29" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="46" t="s">
+      <c r="J29" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="41">
+      <c r="K29" s="26">
         <v>8</v>
       </c>
-      <c r="L29" s="45" t="s">
+      <c r="L29" s="28" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D8:D20"/>
+    <mergeCell ref="E8:E20"/>
+    <mergeCell ref="I8:I12"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="L8:L12"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="K19:K20"/>
@@ -1737,22 +1754,14 @@
     <mergeCell ref="J22:J25"/>
     <mergeCell ref="K22:K25"/>
     <mergeCell ref="L22:L25"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="D8:D20"/>
-    <mergeCell ref="E8:E20"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="K8:K12"/>
-    <mergeCell ref="L8:L12"/>
-    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K11 K13:K14 K16 K19:K22 K26 K28:K29" xr:uid="{7C6B0A2E-68C0-489C-B751-32CFC830261F}">

</xml_diff>